<commit_message>
Update with new markdown content.
</commit_message>
<xml_diff>
--- a/assets/examples/xlsx/RS0006ExampleFile-constefficiency.a205.xlsx
+++ b/assets/examples/xlsx/RS0006ExampleFile-constefficiency.a205.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,24 +28,57 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="00FFFFFF"/>
       <sz val="14"/>
     </font>
     <font>
       <b val="1"/>
     </font>
+    <font/>
     <font>
+      <b val="1"/>
       <color rgb="000070C0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00808B96"/>
+        <bgColor rgb="00808B96"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000529B"/>
+        <bgColor rgb="0000529B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0001AED8"/>
+        <bgColor rgb="0001AED8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9D9D9"/>
+        <bgColor rgb="00D9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -53,27 +86,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0"/>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0"/>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0"/>
+    <xf borderId="1" fillId="6" fontId="3" numFmtId="0"/>
+    <xf borderId="1" fillId="5" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf borderId="1" fillId="6" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment textRotation="45"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment textRotation="45"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle hidden="0" name="Title" xfId="1"/>
+    <cellStyle hidden="0" name="Heading" xfId="2"/>
+    <cellStyle hidden="0" name="Schema" xfId="3"/>
+    <cellStyle hidden="0" name="Value" xfId="4"/>
+    <cellStyle hidden="0" name="Grid Variables" xfId="5"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -85,79 +146,104 @@
     <author>ASHRAE 205</author>
   </authors>
   <commentList>
+    <comment authorId="0" ref="B3" shapeId="0">
+      <text>
+        <t>ASHRAE 205 standard version</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="B4" shapeId="0">
       <text>
-        <t>ASHRAE 205 standard version</t>
+        <t>ASHRAE 205 schema version</t>
       </text>
     </comment>
     <comment authorId="0" ref="B5" shapeId="0">
       <text>
-        <t>ASHRAE 205 schema version</t>
+        <t>Representation specification identifier</t>
       </text>
     </comment>
     <comment authorId="0" ref="B6" shapeId="0">
       <text>
-        <t>Representation specification identifier</t>
+        <t>Free-form description of equipment (suitable for display)</t>
       </text>
     </comment>
     <comment authorId="0" ref="B7" shapeId="0">
       <text>
-        <t>Free-form description of equipment (suitable for display)</t>
+        <t>Unique equipment identifier</t>
       </text>
     </comment>
     <comment authorId="0" ref="B8" shapeId="0">
       <text>
-        <t>Unique equipment identifier</t>
+        <t>Date of publication</t>
       </text>
     </comment>
     <comment authorId="0" ref="B9" shapeId="0">
       <text>
-        <t>Date of publication</t>
+        <t>Integer version identifier for the data in the representation</t>
       </text>
     </comment>
     <comment authorId="0" ref="B10" shapeId="0">
       <text>
-        <t>Integer version identifier for the data in the representation</t>
+        <t>Free-form identification of the source of this data</t>
       </text>
     </comment>
     <comment authorId="0" ref="B11" shapeId="0">
       <text>
-        <t>Free-form identification of the source of this data</t>
+        <t>Free-form characterization of accuracy, limitations, and applicability of this data</t>
       </text>
     </comment>
     <comment authorId="0" ref="B12" shapeId="0">
       <text>
-        <t>Free-form characterization of accuracy, limitations, and applicability of this data</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="B13" shapeId="0">
-      <text>
         <t>Additional Information</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A16" shapeId="0">
+    <comment authorId="0" ref="A13" shapeId="0">
+      <text>
+        <t>*Representation Specification* Data Group</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A14" shapeId="0">
+      <text>
+        <t>Data group describing product and rating information</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A15" shapeId="0">
       <text>
         <t>Data group describing product information</t>
       </text>
     </comment>
+    <comment authorId="0" ref="B16" shapeId="0">
+      <text>
+        <t>Name of the manufacturer</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="B17" shapeId="0">
       <text>
-        <t>Name of the manufacturer</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="B18" shapeId="0">
-      <text>
         <t>Model number for this chiller</t>
       </text>
     </comment>
+    <comment authorId="0" ref="A18" shapeId="0">
+      <text>
+        <t>Data group containing performance information</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B19" shapeId="0">
+      <text>
+        <t>Maximum operational input power to the motor</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="B20" shapeId="0">
       <text>
-        <t>Maximum operational input power to the motor</t>
+        <t>Continuous unit power draw regardless of whether the fan or DX system are operating.</t>
       </text>
     </comment>
     <comment authorId="0" ref="B21" shapeId="0">
       <text>
-        <t>Continuous unit power draw regardless of whether the fan or DX system are operating.</t>
+        <t>Method used to cool the electronic drive.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A22" shapeId="0">
+      <text>
+        <t>Data group describing fan performance when operating</t>
       </text>
     </comment>
   </commentList>
@@ -483,7 +569,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:AZ22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,352 +577,486 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="2" min="2" width="50"/>
-    <col customWidth="1" max="3" min="3" width="31"/>
+    <col customWidth="1" max="1" min="1" style="1" width="13"/>
+    <col customWidth="1" max="2" min="2" style="1" width="50"/>
+    <col customWidth="1" max="3" min="3" style="1" width="31"/>
+    <col customWidth="1" max="4" min="4" style="1" width="13"/>
+    <col customWidth="1" max="5" min="5" style="1" width="13"/>
+    <col customWidth="1" max="6" min="6" style="1" width="13"/>
+    <col customWidth="1" max="7" min="7" style="1" width="13"/>
+    <col customWidth="1" max="8" min="8" style="1" width="13"/>
+    <col customWidth="1" max="9" min="9" style="1" width="13"/>
+    <col customWidth="1" max="10" min="10" style="1" width="13"/>
+    <col customWidth="1" max="11" min="11" style="1" width="13"/>
+    <col customWidth="1" max="12" min="12" style="1" width="13"/>
+    <col customWidth="1" max="13" min="13" style="1" width="13"/>
+    <col customWidth="1" max="14" min="14" style="1" width="13"/>
+    <col customWidth="1" max="15" min="15" style="1" width="13"/>
+    <col customWidth="1" max="16" min="16" style="1" width="13"/>
+    <col customWidth="1" max="17" min="17" style="1" width="13"/>
+    <col customWidth="1" max="18" min="18" style="1" width="13"/>
+    <col customWidth="1" max="19" min="19" style="1" width="13"/>
+    <col customWidth="1" max="20" min="20" style="1" width="13"/>
+    <col customWidth="1" max="21" min="21" style="1" width="13"/>
+    <col customWidth="1" max="22" min="22" style="1" width="13"/>
+    <col customWidth="1" max="23" min="23" style="1" width="13"/>
+    <col customWidth="1" max="24" min="24" style="1" width="13"/>
+    <col customWidth="1" max="25" min="25" style="1" width="13"/>
+    <col customWidth="1" max="26" min="26" style="1" width="13"/>
+    <col customWidth="1" max="27" min="27" style="1" width="13"/>
+    <col customWidth="1" max="28" min="28" style="1" width="13"/>
+    <col customWidth="1" max="29" min="29" style="1" width="13"/>
+    <col customWidth="1" max="30" min="30" style="1" width="13"/>
+    <col customWidth="1" max="31" min="31" style="1" width="13"/>
+    <col customWidth="1" max="32" min="32" style="1" width="13"/>
+    <col customWidth="1" max="33" min="33" style="1" width="13"/>
+    <col customWidth="1" max="34" min="34" style="1" width="13"/>
+    <col customWidth="1" max="35" min="35" style="1" width="13"/>
+    <col customWidth="1" max="36" min="36" style="1" width="13"/>
+    <col customWidth="1" max="37" min="37" style="1" width="13"/>
+    <col customWidth="1" max="38" min="38" style="1" width="13"/>
+    <col customWidth="1" max="39" min="39" style="1" width="13"/>
+    <col customWidth="1" max="40" min="40" style="1" width="13"/>
+    <col customWidth="1" max="41" min="41" style="1" width="13"/>
+    <col customWidth="1" max="42" min="42" style="1" width="13"/>
+    <col customWidth="1" max="43" min="43" style="1" width="13"/>
+    <col customWidth="1" max="44" min="44" style="1" width="13"/>
+    <col customWidth="1" max="45" min="45" style="1" width="13"/>
+    <col customWidth="1" max="46" min="46" style="1" width="13"/>
+    <col customWidth="1" max="47" min="47" style="1" width="13"/>
+    <col customWidth="1" max="48" min="48" style="1" width="13"/>
+    <col customWidth="1" max="49" min="49" style="1" width="13"/>
+    <col customWidth="1" max="50" min="50" style="1" width="13"/>
+    <col customWidth="1" max="51" min="51" style="1" width="13"/>
+    <col customWidth="1" max="52" min="52" style="1" width="13"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>RS0006: Electronic Motor Drive</t>
         </is>
       </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
+      <c r="U1" s="2" t="n"/>
+      <c r="V1" s="2" t="n"/>
+      <c r="W1" s="2" t="n"/>
+      <c r="X1" s="2" t="n"/>
+      <c r="Y1" s="2" t="n"/>
+      <c r="Z1" s="2" t="n"/>
+      <c r="AA1" s="2" t="n"/>
+      <c r="AB1" s="2" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
+      <c r="AE1" s="2" t="n"/>
+      <c r="AF1" s="2" t="n"/>
+      <c r="AG1" s="2" t="n"/>
+      <c r="AH1" s="2" t="n"/>
+      <c r="AI1" s="2" t="n"/>
+      <c r="AJ1" s="2" t="n"/>
+      <c r="AK1" s="2" t="n"/>
+      <c r="AL1" s="2" t="n"/>
+      <c r="AM1" s="2" t="n"/>
+      <c r="AN1" s="2" t="n"/>
+      <c r="AO1" s="2" t="n"/>
+      <c r="AP1" s="2" t="n"/>
+      <c r="AQ1" s="2" t="n"/>
+      <c r="AR1" s="2" t="n"/>
+      <c r="AS1" s="2" t="n"/>
+      <c r="AT1" s="2" t="n"/>
+      <c r="AU1" s="2" t="n"/>
+      <c r="AV1" s="2" t="n"/>
+      <c r="AW1" s="2" t="n"/>
+      <c r="AX1" s="2" t="n"/>
+      <c r="AY1" s="2" t="n"/>
+      <c r="AZ1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Data Group</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Data Element</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>Units</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>Required</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ASHRAE205</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="A3" s="4" t="n"/>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>standard_version</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>PPR2</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n"/>
+      <c r="E3" s="6" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>standard_version</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>PPR2</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
+      <c r="A4" s="4" t="n"/>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>schema_version</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n"/>
+      <c r="E4" s="6" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>schema_version</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
+      <c r="A5" s="4" t="n"/>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>RS_ID</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>RS0006</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n"/>
+      <c r="E5" s="6" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>RS_ID</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>RS0006</t>
-        </is>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
+      <c r="A6" s="4" t="n"/>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>Electronic Motor Drive</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n"/>
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Electronic Motor Drive</t>
-        </is>
-      </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="A7" s="4" t="n"/>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>bcf8b859-67a3-42f4-8f8d-4e57af1ccf22</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n"/>
+      <c r="E7" s="6" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>bcf8b859-67a3-42f4-8f8d-4e57af1ccf22</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="A8" s="4" t="n"/>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>data_timestamp</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>2020-04-08T00:00Z</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n"/>
+      <c r="E8" s="6" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>data_timestamp</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2020-04-08T00:00Z</t>
-        </is>
-      </c>
-      <c r="E9" s="3" t="inlineStr">
+      <c r="A9" s="4" t="n"/>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>data_version</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="n"/>
+      <c r="E9" s="6" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>data_version</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3" t="inlineStr">
+      <c r="A10" s="4" t="n"/>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>data_source</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>MotorSelect</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n"/>
+      <c r="E10" s="6" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n"/>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>disclaimer</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>Example file - not for simulation</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n"/>
+      <c r="E11" s="6" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n"/>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>This is a JSON version of the sample RS0006 file</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n"/>
+      <c r="E12" s="6" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="inlineStr">
+        <is>
+          <t>RS_instance</t>
+        </is>
+      </c>
+      <c r="B13" s="4" t="n"/>
+      <c r="C13" s="5" t="n"/>
+      <c r="D13" s="4" t="n"/>
+      <c r="E13" s="6" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>data_source</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>MotorSelect</t>
-        </is>
-      </c>
-      <c r="E11" s="3" t="n"/>
-    </row>
-    <row r="12">
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>disclaimer</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Example file - not for simulation</t>
-        </is>
-      </c>
-      <c r="E12" s="3" t="n"/>
-    </row>
-    <row r="13">
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>This is a JSON version of the sample RS0006 file</t>
-        </is>
-      </c>
-      <c r="E13" s="3" t="n"/>
-    </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>ASHRAE205.RS_instance</t>
-        </is>
-      </c>
-      <c r="E14" s="3" t="inlineStr">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>RS_instance.description</t>
+        </is>
+      </c>
+      <c r="B14" s="4" t="n"/>
+      <c r="C14" s="5" t="n"/>
+      <c r="D14" s="4" t="n"/>
+      <c r="E14" s="6" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t>RS_instance.description.product_information</t>
+        </is>
+      </c>
+      <c r="B15" s="4" t="n"/>
+      <c r="C15" s="5" t="n"/>
+      <c r="D15" s="4" t="n"/>
+      <c r="E15" s="6" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n"/>
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">        manufacturer</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>DrivesRUs</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n"/>
+      <c r="E16" s="6" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>ASHRAE205.RS_instance.description</t>
-        </is>
-      </c>
-      <c r="E15" s="3" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>ASHRAE205.RS_instance.description.product_information</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="n"/>
-    </row>
     <row r="17">
-      <c r="B17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">            manufacturer</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>DrivesRUs</t>
-        </is>
-      </c>
-      <c r="E17" s="3" t="inlineStr">
+      <c r="A17" s="4" t="n"/>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">        model_number</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>5791</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n"/>
+      <c r="E17" s="6" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">            model_number</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>5791</t>
-        </is>
-      </c>
-      <c r="E18" s="3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>RS_instance.performance</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="n"/>
+      <c r="C18" s="5" t="n"/>
+      <c r="D18" s="4" t="n"/>
+      <c r="E18" s="6" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>ASHRAE205.RS_instance.performance</t>
-        </is>
-      </c>
-      <c r="E19" s="3" t="n"/>
+      <c r="A19" s="4" t="n"/>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    maximum_power</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D19" s="4" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E19" s="6" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        maximum_power</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>10000</v>
-      </c>
-      <c r="D20" t="inlineStr">
+      <c r="A20" s="4" t="n"/>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    standby_power</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D20" s="4" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="E20" s="3" t="n"/>
+      <c r="E20" s="6" t="n"/>
     </row>
     <row r="21">
-      <c r="B21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        standby_power</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>10</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="E21" s="3" t="n"/>
+      <c r="A21" s="4" t="n"/>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    cooling_method</t>
+        </is>
+      </c>
+      <c r="C21" s="5" t="inlineStr">
+        <is>
+          <t>PASSIVE_COOLED</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n"/>
+      <c r="E21" s="6" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        cooling_method</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>PASSIVE_COOLED</t>
-        </is>
-      </c>
-      <c r="E22" s="3" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>ASHRAE205.RS_instance.performance.performance_map</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
+      <c r="A22" s="4" t="inlineStr">
+        <is>
+          <t>RS_instance.performance.performance_map</t>
+        </is>
+      </c>
+      <c r="B22" s="4" t="n"/>
+      <c r="C22" s="5" t="inlineStr">
         <is>
           <t>$performance_map</t>
         </is>
       </c>
-      <c r="E23" s="3" t="n"/>
+      <c r="D22" s="4" t="n"/>
+      <c r="E22" s="6" t="n"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C4" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C3" type="list">
       <formula1>"PPR2"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C6" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C5" type="list">
       <formula1>"RS0001,RS0002,RS0003,RS0004,RS0005,RS0006"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C22" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C21" type="list">
       <formula1>"PASSIVE_COOLED,ACTIVE_AIR_COOLED,ACTIVE_LIQUID_COOLED"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C22" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <legacyDrawing r:id="anysvml"/>
 </worksheet>
@@ -848,70 +1068,175 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:AZ6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="1" width="13"/>
+    <col customWidth="1" max="2" min="2" style="1" width="13"/>
+    <col customWidth="1" max="3" min="3" style="1" width="13"/>
+    <col customWidth="1" max="4" min="4" style="1" width="13"/>
+    <col customWidth="1" max="5" min="5" style="1" width="13"/>
+    <col customWidth="1" max="6" min="6" style="1" width="13"/>
+    <col customWidth="1" max="7" min="7" style="1" width="13"/>
+    <col customWidth="1" max="8" min="8" style="1" width="13"/>
+    <col customWidth="1" max="9" min="9" style="1" width="13"/>
+    <col customWidth="1" max="10" min="10" style="1" width="13"/>
+    <col customWidth="1" max="11" min="11" style="1" width="13"/>
+    <col customWidth="1" max="12" min="12" style="1" width="13"/>
+    <col customWidth="1" max="13" min="13" style="1" width="13"/>
+    <col customWidth="1" max="14" min="14" style="1" width="13"/>
+    <col customWidth="1" max="15" min="15" style="1" width="13"/>
+    <col customWidth="1" max="16" min="16" style="1" width="13"/>
+    <col customWidth="1" max="17" min="17" style="1" width="13"/>
+    <col customWidth="1" max="18" min="18" style="1" width="13"/>
+    <col customWidth="1" max="19" min="19" style="1" width="13"/>
+    <col customWidth="1" max="20" min="20" style="1" width="13"/>
+    <col customWidth="1" max="21" min="21" style="1" width="13"/>
+    <col customWidth="1" max="22" min="22" style="1" width="13"/>
+    <col customWidth="1" max="23" min="23" style="1" width="13"/>
+    <col customWidth="1" max="24" min="24" style="1" width="13"/>
+    <col customWidth="1" max="25" min="25" style="1" width="13"/>
+    <col customWidth="1" max="26" min="26" style="1" width="13"/>
+    <col customWidth="1" max="27" min="27" style="1" width="13"/>
+    <col customWidth="1" max="28" min="28" style="1" width="13"/>
+    <col customWidth="1" max="29" min="29" style="1" width="13"/>
+    <col customWidth="1" max="30" min="30" style="1" width="13"/>
+    <col customWidth="1" max="31" min="31" style="1" width="13"/>
+    <col customWidth="1" max="32" min="32" style="1" width="13"/>
+    <col customWidth="1" max="33" min="33" style="1" width="13"/>
+    <col customWidth="1" max="34" min="34" style="1" width="13"/>
+    <col customWidth="1" max="35" min="35" style="1" width="13"/>
+    <col customWidth="1" max="36" min="36" style="1" width="13"/>
+    <col customWidth="1" max="37" min="37" style="1" width="13"/>
+    <col customWidth="1" max="38" min="38" style="1" width="13"/>
+    <col customWidth="1" max="39" min="39" style="1" width="13"/>
+    <col customWidth="1" max="40" min="40" style="1" width="13"/>
+    <col customWidth="1" max="41" min="41" style="1" width="13"/>
+    <col customWidth="1" max="42" min="42" style="1" width="13"/>
+    <col customWidth="1" max="43" min="43" style="1" width="13"/>
+    <col customWidth="1" max="44" min="44" style="1" width="13"/>
+    <col customWidth="1" max="45" min="45" style="1" width="13"/>
+    <col customWidth="1" max="46" min="46" style="1" width="13"/>
+    <col customWidth="1" max="47" min="47" style="1" width="13"/>
+    <col customWidth="1" max="48" min="48" style="1" width="13"/>
+    <col customWidth="1" max="49" min="49" style="1" width="13"/>
+    <col customWidth="1" max="50" min="50" style="1" width="13"/>
+    <col customWidth="1" max="51" min="51" style="1" width="13"/>
+    <col customWidth="1" max="52" min="52" style="1" width="13"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ASHRAE205.RS_instance.performance.performance_map.grid_variables</t>
-        </is>
-      </c>
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>RS_instance.performance.performance_map</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
+      <c r="U1" s="2" t="n"/>
+      <c r="V1" s="2" t="n"/>
+      <c r="W1" s="2" t="n"/>
+      <c r="X1" s="2" t="n"/>
+      <c r="Y1" s="2" t="n"/>
+      <c r="Z1" s="2" t="n"/>
+      <c r="AA1" s="2" t="n"/>
+      <c r="AB1" s="2" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
+      <c r="AE1" s="2" t="n"/>
+      <c r="AF1" s="2" t="n"/>
+      <c r="AG1" s="2" t="n"/>
+      <c r="AH1" s="2" t="n"/>
+      <c r="AI1" s="2" t="n"/>
+      <c r="AJ1" s="2" t="n"/>
+      <c r="AK1" s="2" t="n"/>
+      <c r="AL1" s="2" t="n"/>
+      <c r="AM1" s="2" t="n"/>
+      <c r="AN1" s="2" t="n"/>
+      <c r="AO1" s="2" t="n"/>
+      <c r="AP1" s="2" t="n"/>
+      <c r="AQ1" s="2" t="n"/>
+      <c r="AR1" s="2" t="n"/>
+      <c r="AS1" s="2" t="n"/>
+      <c r="AT1" s="2" t="n"/>
+      <c r="AU1" s="2" t="n"/>
+      <c r="AV1" s="2" t="n"/>
+      <c r="AW1" s="2" t="n"/>
+      <c r="AX1" s="2" t="n"/>
+      <c r="AY1" s="2" t="n"/>
+      <c r="AZ1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="inlineStr">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>grid_variables</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>lookup_variables</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="inlineStr">
+      <c r="A3" s="8" t="inlineStr">
         <is>
           <t>output_power</t>
         </is>
       </c>
-      <c r="B3" s="6" t="inlineStr">
+      <c r="B3" s="9" t="inlineStr">
         <is>
           <t>efficiency</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="7" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="5" t="n">
         <v>4052</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.985</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="5" t="n">
         <v>8105</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.985</v>
       </c>
     </row>

</xml_diff>